<commit_message>
Casos de prueba agregados
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/8.xlsx
+++ b/Producto/Web/Casos de prueba/8.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -103,22 +103,16 @@
     <t>Hay playas de estacionamiento cargadas en la Base de Datos para la ciudad "Córdoba"</t>
   </si>
   <si>
-    <t>"Colon" es una direccion valida para la ciudad "Córdoba"</t>
-  </si>
-  <si>
-    <t>"9" es una numeracion valida para la calle "Colon"</t>
-  </si>
-  <si>
-    <t>Ingreso "Córrdoba" en el campo nombre de ciudad</t>
-  </si>
-  <si>
     <t>Se carga la pagina BuscarPlayas, con todas las playas de "Córdoba" disponibles en un mapa. Se carga la informacion de las playas en la grilla de playas debajo del mapa.</t>
   </si>
   <si>
-    <t>Ingreso "Colon" en el campo direccion</t>
-  </si>
-  <si>
     <t>Ingreso "9" en el campo numero</t>
+  </si>
+  <si>
+    <t>Ingreso "Córdoba" en el campo nombre de ciudad</t>
+  </si>
+  <si>
+    <t>Ingreso "Colon" en el campo calle</t>
   </si>
 </sst>
 </file>
@@ -675,10 +669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -704,22 +698,6 @@
       </c>
       <c r="B2" s="8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -735,7 +713,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -787,7 +765,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -796,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="8"/>
     </row>
@@ -805,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="8"/>
     </row>

</xml_diff>